<commit_message>
refactor: update cell indexing in editCustomer and saveCustomer functions for correct data mapping
</commit_message>
<xml_diff>
--- a/app/VehicleDetails/templates/vehicle_upload_template.xlsx
+++ b/app/VehicleDetails/templates/vehicle_upload_template.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MCA Project\github\nnx\app\VehicleDetails\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6E417F-2FCF-45DC-A313-91CA5014954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>LicensePlateNumber</t>
   </si>
@@ -53,13 +59,21 @@
   </si>
   <si>
     <t>ServiceDueDate</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>VehicleType</t>
+  </si>
+  <si>
+    <t>NumberOfSeatsContainer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,12 +99,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe2e8f0"/>
+        <fgColor rgb="FFE2E8F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd6dce5"/>
+        <fgColor rgb="FFD6DCE5"/>
       </patternFill>
     </fill>
   </fills>
@@ -104,31 +118,31 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </right>
       <top style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -136,29 +150,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -169,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -210,71 +224,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -302,7 +316,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -325,11 +339,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -338,13 +352,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -354,7 +368,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -363,7 +377,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -372,7 +386,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -380,10 +394,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -448,69 +462,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="57" customFormat="1" s="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add slow and normal speed limit fields to vehicle details and upload functionality
</commit_message>
<xml_diff>
--- a/app/VehicleDetails/templates/vehicle_upload_template.xlsx
+++ b/app/VehicleDetails/templates/vehicle_upload_template.xlsx
@@ -1,36 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MCA Project\github\nnx\app\VehicleDetails\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6E417F-2FCF-45DC-A313-91CA5014954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>LicensePlateNumber</t>
   </si>
   <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
     <t>IMEI</t>
   </si>
   <si>
     <t>SIM</t>
   </si>
   <si>
+    <t>VehicleType</t>
+  </si>
+  <si>
+    <t>NumberOfSeatsContainer</t>
+  </si>
+  <si>
     <t>VehicleModel</t>
   </si>
   <si>
@@ -61,19 +64,17 @@
     <t>ServiceDueDate</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>VehicleType</t>
-  </si>
-  <si>
-    <t>NumberOfSeatsContainer</t>
+    <t>SlowSpeed</t>
+  </si>
+  <si>
+    <t>NormalSpeed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,12 +100,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2E8F0"/>
+        <fgColor rgb="FFe2e8f0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6DCE5"/>
+        <fgColor rgb="FFd6dce5"/>
       </patternFill>
     </fill>
   </fills>
@@ -118,31 +119,31 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </left>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </right>
       <top style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -150,29 +151,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -183,10 +184,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -224,71 +225,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -316,7 +317,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -339,11 +340,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -352,13 +353,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -368,7 +369,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -377,7 +378,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -386,7 +387,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -394,10 +395,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -462,82 +463,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add insurance expiry field to vehicle details and update related functionalities
</commit_message>
<xml_diff>
--- a/app/VehicleDetails/templates/vehicle_upload_template.xlsx
+++ b/app/VehicleDetails/templates/vehicle_upload_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>LicensePlateNumber</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>InsuranceNumber</t>
+  </si>
+  <si>
+    <t>InsuranceExpiry</t>
   </si>
   <si>
     <t>DriverName</t>
@@ -467,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -484,13 +487,14 @@
     <col min="9" max="9" style="4" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="4" width="15.719285714285713" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="4" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="39.75" customFormat="1" s="1">
@@ -527,7 +531,7 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -547,6 +551,9 @@
       </c>
       <c r="R1" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update vehicle upload template with new formatting
</commit_message>
<xml_diff>
--- a/app/VehicleDetails/templates/vehicle_upload_template.xlsx
+++ b/app/VehicleDetails/templates/vehicle_upload_template.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MCA Project\github\nnx\app\VehicleDetails\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815FA21-F4F2-4ED5-9B94-39A0C0F59337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="408" yWindow="2688" windowWidth="22632" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -67,18 +73,17 @@
     <t>ServiceDueDate</t>
   </si>
   <si>
-    <t>SlowSpeed</t>
-  </si>
-  <si>
-    <t>NormalSpeed</t>
+    <t>slowSpeed</t>
+  </si>
+  <si>
+    <t>normalSpeed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +93,12 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -103,12 +114,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe2e8f0"/>
+        <fgColor rgb="FFE2E8F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd6dce5"/>
+        <fgColor rgb="FFD6DCE5"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,31 +133,31 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </right>
       <top style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -154,29 +165,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -187,10 +203,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -228,71 +244,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -320,7 +336,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -343,11 +359,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -356,13 +372,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -372,7 +388,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -381,7 +397,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -390,7 +406,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -398,10 +414,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -466,48 +482,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="39.75" customFormat="1" s="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -555,8 +569,12 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="2" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: refine vehicle upload validation and error messaging
</commit_message>
<xml_diff>
--- a/app/VehicleDetails/templates/vehicle_upload_template.xlsx
+++ b/app/VehicleDetails/templates/vehicle_upload_template.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MCA Project\github\nnx\app\VehicleDetails\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3815FA21-F4F2-4ED5-9B94-39A0C0F59337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="2688" windowWidth="22632" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -82,7 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,16 +109,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2E8F0"/>
+        <fgColor rgb="FFe2e8f0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6DCE5"/>
+        <fgColor rgb="FFd6dce5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,32 +128,39 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </left>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </right>
       <top style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFcccccc"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -166,33 +168,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -203,10 +206,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -244,71 +247,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,7 +339,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -359,11 +362,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -372,13 +375,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -388,7 +391,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -397,7 +400,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -406,7 +409,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -414,10 +417,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -482,46 +485,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="39.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -570,11 +575,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="C2" s="6"/>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="23.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>